<commit_message>
Agregar imagenes y fuentes de informacion
</commit_message>
<xml_diff>
--- a/proyecto/Cambiosuperficiebosque_2000_2005.xlsx
+++ b/proyecto/Cambiosuperficiebosque_2000_2005.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Usuario\Documents\PARES\SIPARES\CHEMONICS\BD_visualizaciones\DEFORESTACION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W540\Desktop\Maestria\visualanalytic\proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="43">
   <si>
     <t>DEPARTAMENTOS</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t>Vichada</t>
+  </si>
+  <si>
+    <t>Rango</t>
+  </si>
+  <si>
+    <t>2000-2005</t>
   </si>
 </sst>
 </file>
@@ -162,6 +168,7 @@
       <sz val="10"/>
       <color indexed="9"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -177,7 +184,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -200,17 +207,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="30"/>
+      </left>
+      <right style="thin">
+        <color indexed="30"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -535,9 +556,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C193"/>
+  <dimension ref="A1:D193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D193"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -546,7 +569,7 @@
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -556,8 +579,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -567,8 +593,11 @@
       <c r="C2" s="2">
         <v>10656768</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -578,8 +607,11 @@
       <c r="C3" s="2">
         <v>22857</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -589,8 +621,11 @@
       <c r="C4" s="2">
         <v>4571</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -600,8 +635,11 @@
       <c r="C5" s="2">
         <v>231714</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -611,8 +649,11 @@
       <c r="C6" s="2">
         <v>2557</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -622,8 +663,11 @@
       <c r="C7" s="2">
         <v>3195</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -633,8 +677,11 @@
       <c r="C8" s="2">
         <v>2142077</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -644,8 +691,11 @@
       <c r="C9" s="2">
         <v>79854</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -655,8 +705,11 @@
       <c r="C10" s="2">
         <v>15971</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -666,8 +719,11 @@
       <c r="C11" s="2">
         <v>3633202</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -677,8 +733,11 @@
       <c r="C12" s="2">
         <v>63765</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -688,8 +747,11 @@
       <c r="C13" s="2">
         <v>399937</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -699,8 +761,11 @@
       <c r="C14" s="2">
         <v>375275</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -710,8 +775,11 @@
       <c r="C15" s="2">
         <v>31387</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -721,8 +789,11 @@
       <c r="C16" s="2">
         <v>6277</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
@@ -732,8 +803,11 @@
       <c r="C17" s="2">
         <v>1852078</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
@@ -743,8 +817,11 @@
       <c r="C18" s="2">
         <v>22211</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>11</v>
       </c>
@@ -754,8 +831,11 @@
       <c r="C19" s="2">
         <v>105641</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
@@ -765,8 +845,11 @@
       <c r="C20" s="2">
         <v>6403</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>12</v>
       </c>
@@ -776,8 +859,11 @@
       <c r="C21" s="2">
         <v>5219</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
@@ -787,8 +873,11 @@
       <c r="C22" s="2">
         <v>1044</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
@@ -798,8 +887,11 @@
       <c r="C23" s="2">
         <v>317495</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
@@ -809,8 +901,11 @@
       <c r="C24" s="2">
         <v>201</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -820,8 +915,11 @@
       <c r="C25" s="2">
         <v>1782</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -831,8 +929,11 @@
       <c r="C26" s="2">
         <v>7128</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -842,8 +943,11 @@
       <c r="C27" s="2">
         <v>294</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>13</v>
       </c>
@@ -853,8 +957,11 @@
       <c r="C28" s="2">
         <v>59</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
@@ -864,8 +971,11 @@
       <c r="C29" s="2">
         <v>153154</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>13</v>
       </c>
@@ -875,8 +985,11 @@
       <c r="C30" s="2">
         <v>1041</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>13</v>
       </c>
@@ -886,8 +999,11 @@
       <c r="C31" s="2">
         <v>2437</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>14</v>
       </c>
@@ -897,8 +1013,11 @@
       <c r="C32" s="2">
         <v>647041</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>14</v>
       </c>
@@ -908,8 +1027,11 @@
       <c r="C33" s="2">
         <v>67285</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>14</v>
       </c>
@@ -919,8 +1041,11 @@
       <c r="C34" s="2">
         <v>13457</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>14</v>
       </c>
@@ -930,8 +1055,11 @@
       <c r="C35" s="2">
         <v>1822824</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>14</v>
       </c>
@@ -941,8 +1069,11 @@
       <c r="C36" s="2">
         <v>5475</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>14</v>
       </c>
@@ -952,8 +1083,11 @@
       <c r="C37" s="2">
         <v>122990</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>15</v>
       </c>
@@ -963,8 +1097,11 @@
       <c r="C38" s="2">
         <v>503084</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>15</v>
       </c>
@@ -974,8 +1111,11 @@
       <c r="C39" s="2">
         <v>42159</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>15</v>
       </c>
@@ -985,8 +1125,11 @@
       <c r="C40" s="2">
         <v>8432</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>15</v>
       </c>
@@ -996,8 +1139,11 @@
       <c r="C41" s="2">
         <v>1698427</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>15</v>
       </c>
@@ -1007,8 +1153,11 @@
       <c r="C42" s="2">
         <v>6829</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>15</v>
       </c>
@@ -1018,8 +1167,11 @@
       <c r="C43" s="2">
         <v>58960</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>16</v>
       </c>
@@ -1029,8 +1181,11 @@
       <c r="C44" s="2">
         <v>148693</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>16</v>
       </c>
@@ -1040,8 +1195,11 @@
       <c r="C45" s="2">
         <v>11685</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>16</v>
       </c>
@@ -1051,8 +1209,11 @@
       <c r="C46" s="2">
         <v>2337</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>16</v>
       </c>
@@ -1062,8 +1223,11 @@
       <c r="C47" s="2">
         <v>561524</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>16</v>
       </c>
@@ -1073,8 +1237,11 @@
       <c r="C48" s="2">
         <v>3694</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -1084,8 +1251,11 @@
       <c r="C49" s="2">
         <v>16224</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>17</v>
       </c>
@@ -1095,8 +1265,11 @@
       <c r="C50" s="2">
         <v>6936920</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>17</v>
       </c>
@@ -1106,8 +1279,11 @@
       <c r="C51" s="2">
         <v>178537</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>17</v>
       </c>
@@ -1117,8 +1293,11 @@
       <c r="C52" s="2">
         <v>35707</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>17</v>
       </c>
@@ -1128,8 +1307,11 @@
       <c r="C53" s="2">
         <v>1860133</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>17</v>
       </c>
@@ -1139,8 +1321,11 @@
       <c r="C54" s="2">
         <v>13496</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>17</v>
       </c>
@@ -1150,8 +1335,11 @@
       <c r="C55" s="2">
         <v>20189</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -1161,8 +1349,11 @@
       <c r="C56" s="2">
         <v>536890</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
@@ -1172,8 +1363,11 @@
       <c r="C57" s="2">
         <v>35557</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -1183,8 +1377,11 @@
       <c r="C58" s="2">
         <v>7111</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
@@ -1194,8 +1391,11 @@
       <c r="C59" s="2">
         <v>3764630</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>18</v>
       </c>
@@ -1205,8 +1405,11 @@
       <c r="C60" s="2">
         <v>17119</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>18</v>
       </c>
@@ -1216,8 +1419,11 @@
       <c r="C61" s="2">
         <v>94147</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>19</v>
       </c>
@@ -1227,8 +1433,11 @@
       <c r="C62" s="2">
         <v>1503048</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>19</v>
       </c>
@@ -1238,8 +1447,11 @@
       <c r="C63" s="2">
         <v>35202</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>19</v>
       </c>
@@ -1249,8 +1461,11 @@
       <c r="C64" s="2">
         <v>7040</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>19</v>
       </c>
@@ -1260,8 +1475,11 @@
       <c r="C65" s="2">
         <v>1399931</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>19</v>
       </c>
@@ -1271,8 +1489,11 @@
       <c r="C66" s="2">
         <v>10614</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>19</v>
       </c>
@@ -1282,8 +1503,11 @@
       <c r="C67" s="2">
         <v>109955</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
@@ -1293,8 +1517,11 @@
       <c r="C68" s="2">
         <v>178561</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
@@ -1304,8 +1531,11 @@
       <c r="C69" s="2">
         <v>14129</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>20</v>
       </c>
@@ -1315,8 +1545,11 @@
       <c r="C70" s="2">
         <v>2826</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>20</v>
       </c>
@@ -1326,8 +1559,11 @@
       <c r="C71" s="2">
         <v>2019606</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>20</v>
       </c>
@@ -1337,8 +1573,11 @@
       <c r="C72" s="2">
         <v>7999</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>20</v>
       </c>
@@ -1348,8 +1587,11 @@
       <c r="C73" s="2">
         <v>25359</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>21</v>
       </c>
@@ -1359,8 +1601,11 @@
       <c r="C74" s="2">
         <v>3563897</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>21</v>
       </c>
@@ -1370,8 +1615,11 @@
       <c r="C75" s="2">
         <v>56841</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>21</v>
       </c>
@@ -1381,8 +1629,11 @@
       <c r="C76" s="2">
         <v>11368</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>21</v>
       </c>
@@ -1392,8 +1643,11 @@
       <c r="C77" s="2">
         <v>362478</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>21</v>
       </c>
@@ -1403,8 +1657,11 @@
       <c r="C78" s="2">
         <v>56685</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>21</v>
       </c>
@@ -1414,8 +1671,11 @@
       <c r="C79" s="2">
         <v>758597</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -1425,8 +1685,11 @@
       <c r="C80" s="2">
         <v>299709</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>22</v>
       </c>
@@ -1436,8 +1699,11 @@
       <c r="C81" s="2">
         <v>43076</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -1447,8 +1713,11 @@
       <c r="C82" s="2">
         <v>8615</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>22</v>
       </c>
@@ -1458,8 +1727,11 @@
       <c r="C83" s="2">
         <v>1773096</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>22</v>
       </c>
@@ -1469,8 +1741,11 @@
       <c r="C84" s="2">
         <v>12724</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>22</v>
       </c>
@@ -1480,8 +1755,11 @@
       <c r="C85" s="2">
         <v>107533</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>23</v>
       </c>
@@ -1491,8 +1769,11 @@
       <c r="C86" s="2">
         <v>365529</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>23</v>
       </c>
@@ -1502,8 +1783,11 @@
       <c r="C87" s="2">
         <v>13912</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>23</v>
       </c>
@@ -1513,8 +1797,11 @@
       <c r="C88" s="2">
         <v>2782</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>23</v>
       </c>
@@ -1524,8 +1811,11 @@
       <c r="C89" s="2">
         <v>1955517</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>23</v>
       </c>
@@ -1535,8 +1825,11 @@
       <c r="C90" s="2">
         <v>9176</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>23</v>
       </c>
@@ -1546,8 +1839,11 @@
       <c r="C91" s="2">
         <v>159350</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>24</v>
       </c>
@@ -1557,8 +1853,11 @@
       <c r="C92" s="2">
         <v>6652453</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>24</v>
       </c>
@@ -1568,8 +1867,11 @@
       <c r="C93" s="2">
         <v>21875</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>24</v>
       </c>
@@ -1579,8 +1881,11 @@
       <c r="C94" s="2">
         <v>4375</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>24</v>
       </c>
@@ -1590,8 +1895,11 @@
       <c r="C95" s="2">
         <v>450116</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>24</v>
       </c>
@@ -1601,8 +1909,11 @@
       <c r="C96" s="2">
         <v>2992</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>24</v>
       </c>
@@ -1612,8 +1923,11 @@
       <c r="C97" s="2">
         <v>6765</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>25</v>
       </c>
@@ -1623,8 +1937,11 @@
       <c r="C98" s="2">
         <v>4967739</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>25</v>
       </c>
@@ -1634,8 +1951,11 @@
       <c r="C99" s="2">
         <v>78408</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>25</v>
       </c>
@@ -1645,8 +1965,11 @@
       <c r="C100" s="2">
         <v>15682</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>25</v>
       </c>
@@ -1656,8 +1979,11 @@
       <c r="C101" s="2">
         <v>492467</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>25</v>
       </c>
@@ -1667,8 +1993,11 @@
       <c r="C102" s="2">
         <v>4794</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>25</v>
       </c>
@@ -1678,8 +2007,11 @@
       <c r="C103" s="2">
         <v>2743</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>26</v>
       </c>
@@ -1689,8 +2021,11 @@
       <c r="C104" s="2">
         <v>602991</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>26</v>
       </c>
@@ -1700,8 +2035,11 @@
       <c r="C105" s="2">
         <v>60438</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>26</v>
       </c>
@@ -1711,8 +2049,11 @@
       <c r="C106" s="2">
         <v>12088</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>26</v>
       </c>
@@ -1722,8 +2063,11 @@
       <c r="C107" s="2">
         <v>1150701</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>26</v>
       </c>
@@ -1733,8 +2077,11 @@
       <c r="C108" s="2">
         <v>10584</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>26</v>
       </c>
@@ -1744,8 +2091,11 @@
       <c r="C109" s="2">
         <v>47179</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>27</v>
       </c>
@@ -1755,8 +2105,11 @@
       <c r="C110" s="2">
         <v>149861</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>27</v>
       </c>
@@ -1766,8 +2119,11 @@
       <c r="C111" s="2">
         <v>24077</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>27</v>
       </c>
@@ -1777,8 +2133,11 @@
       <c r="C112" s="2">
         <v>4815</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>27</v>
       </c>
@@ -1788,8 +2147,11 @@
       <c r="C113" s="2">
         <v>1810201</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D113" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>27</v>
       </c>
@@ -1799,8 +2161,11 @@
       <c r="C114" s="2">
         <v>11782</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D114" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>27</v>
       </c>
@@ -1810,8 +2175,11 @@
       <c r="C115" s="2">
         <v>69389</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>28</v>
       </c>
@@ -1821,8 +2189,11 @@
       <c r="C116" s="2">
         <v>327586</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D116" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>28</v>
       </c>
@@ -1832,8 +2203,11 @@
       <c r="C117" s="2">
         <v>32308</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D117" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>28</v>
       </c>
@@ -1843,8 +2217,11 @@
       <c r="C118" s="2">
         <v>6462</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D118" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>28</v>
       </c>
@@ -1854,8 +2231,11 @@
       <c r="C119" s="2">
         <v>1925015</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D119" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>28</v>
       </c>
@@ -1865,8 +2245,11 @@
       <c r="C120" s="2">
         <v>22125</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D120" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>28</v>
       </c>
@@ -1876,8 +2259,11 @@
       <c r="C121" s="2">
         <v>13651</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D121" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>29</v>
       </c>
@@ -1887,8 +2273,11 @@
       <c r="C122" s="2">
         <v>3303911</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D122" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>29</v>
       </c>
@@ -1898,8 +2287,11 @@
       <c r="C123" s="2">
         <v>197268</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D123" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>29</v>
       </c>
@@ -1909,8 +2301,11 @@
       <c r="C124" s="2">
         <v>39454</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D124" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>29</v>
       </c>
@@ -1920,8 +2315,11 @@
       <c r="C125" s="2">
         <v>4905767</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D125" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>29</v>
       </c>
@@ -1931,8 +2329,11 @@
       <c r="C126" s="2">
         <v>52717</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D126" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>29</v>
       </c>
@@ -1942,8 +2343,11 @@
       <c r="C127" s="2">
         <v>85845</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D127" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>30</v>
       </c>
@@ -1953,8 +2357,11 @@
       <c r="C128" s="2">
         <v>1735261</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D128" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>30</v>
       </c>
@@ -1964,8 +2371,11 @@
       <c r="C129" s="2">
         <v>136533</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D129" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>30</v>
       </c>
@@ -1975,8 +2385,11 @@
       <c r="C130" s="2">
         <v>27307</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D130" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>30</v>
       </c>
@@ -1986,8 +2399,11 @@
       <c r="C131" s="2">
         <v>940090</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D131" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>30</v>
       </c>
@@ -1997,8 +2413,11 @@
       <c r="C132" s="2">
         <v>21065</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D132" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>30</v>
       </c>
@@ -2008,8 +2427,11 @@
       <c r="C133" s="2">
         <v>304423</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D133" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>31</v>
       </c>
@@ -2019,8 +2441,11 @@
       <c r="C134" s="2">
         <v>944526</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D134" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>31</v>
       </c>
@@ -2030,8 +2455,11 @@
       <c r="C135" s="2">
         <v>61778</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D135" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>31</v>
       </c>
@@ -2041,8 +2469,11 @@
       <c r="C136" s="2">
         <v>12356</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D136" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>31</v>
       </c>
@@ -2052,8 +2483,11 @@
       <c r="C137" s="2">
         <v>1076687</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D137" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>31</v>
       </c>
@@ -2063,8 +2497,11 @@
       <c r="C138" s="2">
         <v>19583</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D138" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>31</v>
       </c>
@@ -2074,8 +2511,11 @@
       <c r="C139" s="2">
         <v>91317</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D139" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>32</v>
       </c>
@@ -2085,8 +2525,11 @@
       <c r="C140" s="2">
         <v>1939005</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D140" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>32</v>
       </c>
@@ -2096,8 +2539,11 @@
       <c r="C141" s="2">
         <v>63301</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D141" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>32</v>
       </c>
@@ -2107,8 +2553,11 @@
       <c r="C142" s="2">
         <v>12660</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D142" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>32</v>
       </c>
@@ -2118,8 +2567,11 @@
       <c r="C143" s="2">
         <v>572734</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D143" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>32</v>
       </c>
@@ -2129,8 +2581,11 @@
       <c r="C144" s="2">
         <v>2690</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D144" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>32</v>
       </c>
@@ -2140,8 +2595,11 @@
       <c r="C145" s="2">
         <v>12348</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D145" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>33</v>
       </c>
@@ -2151,8 +2609,11 @@
       <c r="C146" s="2">
         <v>50181</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D146" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>33</v>
       </c>
@@ -2162,8 +2623,11 @@
       <c r="C147" s="2">
         <v>4237</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D147" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>33</v>
       </c>
@@ -2173,8 +2637,11 @@
       <c r="C148" s="2">
         <v>847</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D148" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>33</v>
       </c>
@@ -2184,8 +2651,11 @@
       <c r="C149" s="2">
         <v>120215</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D149" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>33</v>
       </c>
@@ -2195,8 +2665,11 @@
       <c r="C150" s="2">
         <v>795</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D150" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>33</v>
       </c>
@@ -2206,8 +2679,11 @@
       <c r="C151" s="2">
         <v>18117</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D151" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>34</v>
       </c>
@@ -2217,8 +2693,11 @@
       <c r="C152" s="2">
         <v>136815</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D152" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>34</v>
       </c>
@@ -2228,8 +2707,11 @@
       <c r="C153" s="2">
         <v>5338</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D153" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>34</v>
       </c>
@@ -2239,8 +2721,11 @@
       <c r="C154" s="2">
         <v>1068</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D154" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>34</v>
       </c>
@@ -2250,8 +2735,11 @@
       <c r="C155" s="2">
         <v>181760</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D155" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>34</v>
       </c>
@@ -2261,8 +2749,11 @@
       <c r="C156" s="2">
         <v>2494</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D156" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>34</v>
       </c>
@@ -2272,8 +2763,11 @@
       <c r="C157" s="2">
         <v>26985</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D157" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>35</v>
       </c>
@@ -2283,8 +2777,11 @@
       <c r="C158" s="2">
         <v>846861</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D158" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>35</v>
       </c>
@@ -2294,8 +2791,11 @@
       <c r="C159" s="2">
         <v>87246</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D159" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>35</v>
       </c>
@@ -2305,8 +2805,11 @@
       <c r="C160" s="2">
         <v>17449</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D160" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>35</v>
       </c>
@@ -2316,8 +2819,11 @@
       <c r="C161" s="2">
         <v>1961574</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D161" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>35</v>
       </c>
@@ -2327,8 +2833,11 @@
       <c r="C162" s="2">
         <v>28710</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D162" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>35</v>
       </c>
@@ -2338,8 +2847,11 @@
       <c r="C163" s="2">
         <v>133837</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D163" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>36</v>
       </c>
@@ -2349,8 +2861,11 @@
       <c r="C164" s="2">
         <v>34327</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D164" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>36</v>
       </c>
@@ -2360,8 +2875,11 @@
       <c r="C165" s="2">
         <v>21604</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D165" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>36</v>
       </c>
@@ -2371,8 +2889,11 @@
       <c r="C166" s="2">
         <v>4321</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D166" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>36</v>
       </c>
@@ -2382,8 +2903,11 @@
       <c r="C167" s="2">
         <v>988123</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D167" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>36</v>
       </c>
@@ -2393,8 +2917,11 @@
       <c r="C168" s="2">
         <v>743</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D168" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>36</v>
       </c>
@@ -2404,8 +2931,11 @@
       <c r="C169" s="2">
         <v>26362</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D169" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>37</v>
       </c>
@@ -2415,8 +2945,11 @@
       <c r="C170" s="2">
         <v>467929</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D170" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>37</v>
       </c>
@@ -2426,8 +2959,11 @@
       <c r="C171" s="2">
         <v>53307</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D171" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>37</v>
       </c>
@@ -2437,8 +2973,11 @@
       <c r="C172" s="2">
         <v>10661</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D172" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>37</v>
       </c>
@@ -2448,8 +2987,11 @@
       <c r="C173" s="2">
         <v>1778922</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D173" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>37</v>
       </c>
@@ -2459,8 +3001,11 @@
       <c r="C174" s="2">
         <v>11040</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D174" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>37</v>
       </c>
@@ -2470,8 +3015,11 @@
       <c r="C175" s="2">
         <v>85909</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D175" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>38</v>
       </c>
@@ -2481,8 +3029,11 @@
       <c r="C176" s="2">
         <v>856322</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D176" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>38</v>
       </c>
@@ -2492,8 +3043,11 @@
       <c r="C177" s="2">
         <v>17290</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D177" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>38</v>
       </c>
@@ -2503,8 +3057,11 @@
       <c r="C178" s="2">
         <v>3458</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D178" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>38</v>
       </c>
@@ -2514,8 +3071,11 @@
       <c r="C179" s="2">
         <v>1052607</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D179" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>38</v>
       </c>
@@ -2525,8 +3085,11 @@
       <c r="C180" s="2">
         <v>19288</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D180" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>38</v>
       </c>
@@ -2536,8 +3099,11 @@
       <c r="C181" s="2">
         <v>148961</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D181" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>39</v>
       </c>
@@ -2547,8 +3113,11 @@
       <c r="C182" s="2">
         <v>5183875</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D182" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>39</v>
       </c>
@@ -2558,8 +3127,11 @@
       <c r="C183" s="2">
         <v>19531</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D183" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>39</v>
       </c>
@@ -2569,8 +3141,11 @@
       <c r="C184" s="2">
         <v>3906</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D184" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>39</v>
       </c>
@@ -2580,8 +3155,11 @@
       <c r="C185" s="2">
         <v>138383</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D185" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>39</v>
       </c>
@@ -2591,8 +3169,11 @@
       <c r="C186" s="2">
         <v>2960</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D186" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>39</v>
       </c>
@@ -2602,8 +3183,11 @@
       <c r="C187" s="2">
         <v>3781</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D187" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>40</v>
       </c>
@@ -2613,8 +3197,11 @@
       <c r="C188" s="2">
         <v>4162002</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D188" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>40</v>
       </c>
@@ -2624,8 +3211,11 @@
       <c r="C189" s="2">
         <v>55480</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D189" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>40</v>
       </c>
@@ -2635,8 +3225,11 @@
       <c r="C190" s="2">
         <v>11096</v>
       </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D190" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>40</v>
       </c>
@@ -2646,8 +3239,11 @@
       <c r="C191" s="2">
         <v>5761229</v>
       </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D191" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>40</v>
       </c>
@@ -2657,8 +3253,11 @@
       <c r="C192" s="2">
         <v>9767</v>
       </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D192" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>40</v>
       </c>
@@ -2667,6 +3266,9 @@
       </c>
       <c r="C193" s="2">
         <v>14785</v>
+      </c>
+      <c r="D193" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>